<commit_message>
fix greedy, fix dataset names, make path building take nearest vertex first
</commit_message>
<xml_diff>
--- a/dataset/ГрафДанные.xlsx
+++ b/dataset/ГрафДанные.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\ldt-rosatom\dataset\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0442F385-14B5-4565-8456-016F5AB1CCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
+    <workbookView xWindow="3585" yWindow="4185" windowWidth="25095" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="points" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -104,103 +110,106 @@
     <t>Бухта Север и Диксон</t>
   </si>
   <si>
-    <t>кромка льда на Западе</t>
-  </si>
-  <si>
     <t>Победа месторождение</t>
   </si>
   <si>
-    <t>Карское - 3 (центр)</t>
-  </si>
-  <si>
-    <t>пролив Вилькицкого - 3</t>
-  </si>
-  <si>
-    <t>Лаптевых - 4 (юг)</t>
-  </si>
-  <si>
-    <t>Лаптевых - 1 (центр)</t>
-  </si>
-  <si>
-    <t>Карское - 1 (сбор каравана)</t>
-  </si>
-  <si>
-    <t>остров Врангеля</t>
-  </si>
-  <si>
-    <t>Восточно-Сибирское - 1 (восток)</t>
-  </si>
-  <si>
-    <t>около Новой Земли</t>
-  </si>
-  <si>
-    <t>Пролив Санникова - 1</t>
-  </si>
-  <si>
-    <t>Пролив Санникова - 2</t>
-  </si>
-  <si>
     <t>устье Лены</t>
   </si>
   <si>
-    <t>мыс.Наглёйнын</t>
-  </si>
-  <si>
-    <t>пролив Лонга</t>
-  </si>
-  <si>
-    <t>Восточно-Сибирское - 3 (север)</t>
-  </si>
-  <si>
-    <t>Лаптевых - 3 (восток)</t>
-  </si>
-  <si>
-    <t>Восточно-Сибирское - 2 (запад)</t>
-  </si>
-  <si>
     <t>Ленинградское-Русановское</t>
   </si>
   <si>
-    <t>терминал Утренний</t>
-  </si>
-  <si>
     <t>Таймырский залив</t>
   </si>
   <si>
     <t>Берингово</t>
   </si>
   <si>
-    <t>кромка льда на Востоке</t>
-  </si>
-  <si>
     <t>Рейд Певек</t>
   </si>
   <si>
-    <t>Лаптевых - 2 (центр)</t>
-  </si>
-  <si>
     <t>Рейд Мурманска</t>
   </si>
   <si>
-    <t>остров Котельный</t>
-  </si>
-  <si>
-    <t>Карское - 2 (прибрежный)</t>
-  </si>
-  <si>
     <t>Берингов пролив</t>
   </si>
   <si>
-    <t>пролив Вилькицкого - восток</t>
-  </si>
-  <si>
-    <t>пролив Вилькицкого - запад</t>
+    <t>Кромка льда на Западе</t>
+  </si>
+  <si>
+    <t>Остров Врангеля</t>
+  </si>
+  <si>
+    <t>Около Новой Земли</t>
+  </si>
+  <si>
+    <t>Мыс.Наглёйнын</t>
+  </si>
+  <si>
+    <t>Пролив Лонга</t>
+  </si>
+  <si>
+    <t>Терминал Утренний</t>
+  </si>
+  <si>
+    <t>Кромка льда на Востоке</t>
+  </si>
+  <si>
+    <t>Остров Котельный</t>
+  </si>
+  <si>
+    <t>Восточно-Сибирское 1</t>
+  </si>
+  <si>
+    <t>rep_id обозначение на картинке</t>
+  </si>
+  <si>
+    <t>Карское 3</t>
+  </si>
+  <si>
+    <t>Пролив Вилькицкого 3</t>
+  </si>
+  <si>
+    <t>Лаптевых 4</t>
+  </si>
+  <si>
+    <t>Лаптевых 1</t>
+  </si>
+  <si>
+    <t>Карское 1</t>
+  </si>
+  <si>
+    <t>Пролив Вилькицкого восток</t>
+  </si>
+  <si>
+    <t>Пролив Вилькицкого запад</t>
+  </si>
+  <si>
+    <t>Пролив Санникова 1</t>
+  </si>
+  <si>
+    <t>Пролив Санникова 2</t>
+  </si>
+  <si>
+    <t>Восточно-Сибирское 3</t>
+  </si>
+  <si>
+    <t>Лаптевых 3</t>
+  </si>
+  <si>
+    <t>Восточно-Сибирское 2</t>
+  </si>
+  <si>
+    <t>Лаптевых 2</t>
+  </si>
+  <si>
+    <t>Карское 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -269,6 +278,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -316,7 +328,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,9 +361,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -384,6 +413,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -559,11 +605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +655,7 @@
         <v>1010</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -640,7 +686,7 @@
         <v>44.6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3">
         <v>2002</v>
@@ -708,7 +754,7 @@
         <v>63.9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="3">
         <v>1011</v>
@@ -725,7 +771,7 @@
         <v>86.4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E9" s="3">
         <v>2008</v>
@@ -742,7 +788,7 @@
         <v>107.7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3">
         <v>2013</v>
@@ -759,7 +805,7 @@
         <v>116.7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E11" s="3">
         <v>2018</v>
@@ -810,7 +856,7 @@
         <v>116</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E14" s="3">
         <v>2015</v>
@@ -827,7 +873,7 @@
         <v>76.7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3">
         <v>2006</v>
@@ -895,7 +941,7 @@
         <v>184.7</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E19" s="3">
         <v>2026</v>
@@ -912,7 +958,7 @@
         <v>170.5</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E20" s="3">
         <v>2023</v>
@@ -929,7 +975,7 @@
         <v>104.1</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E21" s="3">
         <v>2012</v>
@@ -946,7 +992,7 @@
         <v>99.5</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E22" s="3">
         <v>2011</v>
@@ -963,7 +1009,7 @@
         <v>58.3</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3">
         <v>2004</v>
@@ -980,7 +1026,7 @@
         <v>139</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E24" s="3">
         <v>2020</v>
@@ -997,7 +1043,7 @@
         <v>146.69999999999999</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E25" s="3">
         <v>2021</v>
@@ -1014,7 +1060,7 @@
         <v>128.1</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3">
         <v>2019</v>
@@ -1048,7 +1094,7 @@
         <v>169.4</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E28" s="3">
         <v>1009</v>
@@ -1065,7 +1111,7 @@
         <v>179</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E29" s="3">
         <v>2027</v>
@@ -1082,7 +1128,7 @@
         <v>169.9</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3">
         <v>2025</v>
@@ -1116,7 +1162,7 @@
         <v>152.6</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E32" s="3">
         <v>2017</v>
@@ -1167,7 +1213,7 @@
         <v>159.5</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E35" s="3">
         <v>2024</v>
@@ -1184,7 +1230,7 @@
         <v>65.599999999999994</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E36" s="3">
         <v>1013</v>
@@ -1201,7 +1247,7 @@
         <v>73.73</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E37" s="3">
         <v>1005</v>
@@ -1218,7 +1264,7 @@
         <v>97.6</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E38" s="3">
         <v>2010</v>
@@ -1235,7 +1281,7 @@
         <v>188.2</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E39" s="3">
         <v>2029</v>
@@ -1252,7 +1298,7 @@
         <v>175.3</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E40" s="3">
         <v>2030</v>
@@ -1269,7 +1315,7 @@
         <v>169.9</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="E41" s="3">
         <v>1006</v>
@@ -1286,7 +1332,7 @@
         <v>131.5</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E42" s="3">
         <v>2016</v>
@@ -1303,7 +1349,7 @@
         <v>33.75</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="E43" s="3">
         <v>1001</v>
@@ -1320,7 +1366,7 @@
         <v>140.80000000000001</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E44" s="3">
         <v>2022</v>
@@ -1337,7 +1383,7 @@
         <v>84.2</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E45" s="3">
         <v>2007</v>
@@ -1371,7 +1417,7 @@
         <v>-169.35</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="E47" s="3">
         <v>2028</v>
@@ -1400,7 +1446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>